<commit_message>
generated from ./SC24/MCB.json at 2494425
</commit_message>
<xml_diff>
--- a/SC24/artifacts/MCB/MCB.xlsx
+++ b/SC24/artifacts/MCB/MCB.xlsx
@@ -10,14 +10,14 @@
     <sheet name="K-Matrix " sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'K-Matrix '!$A$1:$AR$361</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'K-Matrix '!$A$1:$AR$325</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3734" uniqueCount="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3410" uniqueCount="732">
   <si>
     <t>ID</t>
   </si>
@@ -2110,7 +2110,7 @@
     <t>The red channel of LED #1 of the dashboard</t>
   </si>
   <si>
-    <t>0..31</t>
+    <t>0..7</t>
   </si>
   <si>
     <t>LED_1_green</t>
@@ -2177,63 +2177,6 @@
   </si>
   <si>
     <t>The blue channel of LED #4 of the dashboard</t>
-  </si>
-  <si>
-    <t>6C7h</t>
-  </si>
-  <si>
-    <t>DSPACE_dashLedsColorLiteral</t>
-  </si>
-  <si>
-    <t>LED_1_color</t>
-  </si>
-  <si>
-    <t>Dashboard LED #1 color control</t>
-  </si>
-  <si>
-    <t>BLACK</t>
-  </si>
-  <si>
-    <t>RED</t>
-  </si>
-  <si>
-    <t>GREEN</t>
-  </si>
-  <si>
-    <t>BLUE</t>
-  </si>
-  <si>
-    <t>CYAN</t>
-  </si>
-  <si>
-    <t>LIME</t>
-  </si>
-  <si>
-    <t>MAGENTA</t>
-  </si>
-  <si>
-    <t>YELLOW</t>
-  </si>
-  <si>
-    <t>WHITE</t>
-  </si>
-  <si>
-    <t>LED_2_color</t>
-  </si>
-  <si>
-    <t>Dashboard LED #2 color control</t>
-  </si>
-  <si>
-    <t>LED_3_color</t>
-  </si>
-  <si>
-    <t>Dashboard LED #3 color control</t>
-  </si>
-  <si>
-    <t>LED_4_color</t>
-  </si>
-  <si>
-    <t>Dashboard LED #4 color control</t>
   </si>
   <si>
     <t>708h</t>
@@ -2658,7 +2601,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB360"/>
+  <dimension ref="A1:AB324"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -21672,7 +21615,7 @@
         <v>696</v>
       </c>
       <c r="J310" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K310" s="2">
         <v>0</v>
@@ -21721,7 +21664,7 @@
         <v>1</v>
       </c>
       <c r="G311" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H311" s="6" t="s">
         <v>698</v>
@@ -21730,7 +21673,7 @@
         <v>699</v>
       </c>
       <c r="J311" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K311" s="6">
         <v>0</v>
@@ -21776,10 +21719,10 @@
       </c>
       <c r="E312" s="5"/>
       <c r="F312" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G312" s="6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H312" s="6" t="s">
         <v>700</v>
@@ -21788,7 +21731,7 @@
         <v>701</v>
       </c>
       <c r="J312" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K312" s="6">
         <v>0</v>
@@ -21837,7 +21780,7 @@
         <v>2</v>
       </c>
       <c r="G313" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H313" s="6" t="s">
         <v>702</v>
@@ -21846,7 +21789,7 @@
         <v>703</v>
       </c>
       <c r="J313" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K313" s="6">
         <v>0</v>
@@ -21892,7 +21835,7 @@
       </c>
       <c r="E314" s="5"/>
       <c r="F314" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G314" s="6">
         <v>4</v>
@@ -21904,7 +21847,7 @@
         <v>705</v>
       </c>
       <c r="J314" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K314" s="6">
         <v>0</v>
@@ -21950,10 +21893,10 @@
       </c>
       <c r="E315" s="5"/>
       <c r="F315" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G315" s="6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H315" s="6" t="s">
         <v>706</v>
@@ -21962,7 +21905,7 @@
         <v>707</v>
       </c>
       <c r="J315" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K315" s="6">
         <v>0</v>
@@ -22008,10 +21951,10 @@
       </c>
       <c r="E316" s="5"/>
       <c r="F316" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G316" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H316" s="6" t="s">
         <v>708</v>
@@ -22020,7 +21963,7 @@
         <v>709</v>
       </c>
       <c r="J316" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K316" s="6">
         <v>0</v>
@@ -22066,10 +22009,10 @@
       </c>
       <c r="E317" s="5"/>
       <c r="F317" s="6">
+        <v>3</v>
+      </c>
+      <c r="G317" s="6">
         <v>5</v>
-      </c>
-      <c r="G317" s="6">
-        <v>3</v>
       </c>
       <c r="H317" s="6" t="s">
         <v>710</v>
@@ -22078,7 +22021,7 @@
         <v>711</v>
       </c>
       <c r="J317" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K317" s="6">
         <v>0</v>
@@ -22124,7 +22067,7 @@
       </c>
       <c r="E318" s="5"/>
       <c r="F318" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G318" s="6">
         <v>0</v>
@@ -22136,7 +22079,7 @@
         <v>713</v>
       </c>
       <c r="J318" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K318" s="6">
         <v>0</v>
@@ -22182,10 +22125,10 @@
       </c>
       <c r="E319" s="5"/>
       <c r="F319" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G319" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H319" s="6" t="s">
         <v>714</v>
@@ -22194,7 +22137,7 @@
         <v>715</v>
       </c>
       <c r="J319" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K319" s="6">
         <v>0</v>
@@ -22240,10 +22183,10 @@
       </c>
       <c r="E320" s="5"/>
       <c r="F320" s="6">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G320" s="6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H320" s="6" t="s">
         <v>716</v>
@@ -22252,7 +22195,7 @@
         <v>717</v>
       </c>
       <c r="J320" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K320" s="6">
         <v>0</v>
@@ -22298,10 +22241,10 @@
       </c>
       <c r="E321" s="5"/>
       <c r="F321" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G321" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H321" s="6" t="s">
         <v>718</v>
@@ -22310,7 +22253,7 @@
         <v>719</v>
       </c>
       <c r="J321" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K321" s="6">
         <v>0</v>
@@ -22349,10 +22292,10 @@
         <v>721</v>
       </c>
       <c r="C322" s="2">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="D322" s="2" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="E322" s="2"/>
       <c r="F322" s="2">
@@ -22364,11 +22307,9 @@
       <c r="H322" s="2" t="s">
         <v>722</v>
       </c>
-      <c r="I322" s="2" t="s">
-        <v>723</v>
-      </c>
+      <c r="I322" s="2"/>
       <c r="J322" s="2">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="K322" s="2">
         <v>0</v>
@@ -22379,9 +22320,7 @@
       <c r="M322" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N322" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="N322" s="4"/>
       <c r="O322" s="2"/>
       <c r="P322" s="4"/>
       <c r="Q322" s="2"/>
@@ -22392,2293 +22331,137 @@
       <c r="V322" s="4"/>
       <c r="W322" s="2"/>
       <c r="X322" s="4"/>
-      <c r="Y322" s="2"/>
-      <c r="Z322" s="2">
-        <v>0</v>
-      </c>
+      <c r="Y322" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z322" s="2"/>
       <c r="AA322" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB322" s="2"/>
+    </row>
+    <row r="323" spans="1:28">
+      <c r="A323" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="B323" s="2" t="s">
         <v>724</v>
       </c>
-      <c r="AB322" s="2"/>
-    </row>
-    <row r="323" spans="1:28" outlineLevel="1">
-      <c r="A323" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B323" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C323" s="5">
-        <v>200</v>
-      </c>
-      <c r="D323" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E323" s="5"/>
-      <c r="F323" s="5">
-        <v>1</v>
-      </c>
-      <c r="G323" s="5">
-        <v>0</v>
-      </c>
-      <c r="H323" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="I323" s="5" t="s">
-        <v>723</v>
-      </c>
-      <c r="J323" s="5">
-        <v>4</v>
-      </c>
-      <c r="K323" s="5">
-        <v>0</v>
-      </c>
-      <c r="L323" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M323" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N323" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O323" s="6"/>
-      <c r="P323" s="8"/>
-      <c r="Q323" s="6"/>
-      <c r="R323" s="8"/>
-      <c r="S323" s="6"/>
-      <c r="T323" s="8"/>
-      <c r="U323" s="6"/>
-      <c r="V323" s="8"/>
-      <c r="W323" s="6"/>
-      <c r="X323" s="8"/>
-      <c r="Y323" s="6"/>
-      <c r="Z323" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA323" s="6" t="s">
+      <c r="C323" s="2">
+        <v>0</v>
+      </c>
+      <c r="D323" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E323" s="2"/>
+      <c r="F323" s="2">
+        <v>1</v>
+      </c>
+      <c r="G323" s="2">
+        <v>0</v>
+      </c>
+      <c r="H323" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="AB323" s="5"/>
-    </row>
-    <row r="324" spans="1:28" outlineLevel="1">
-      <c r="A324" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B324" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C324" s="5">
-        <v>200</v>
-      </c>
-      <c r="D324" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E324" s="5"/>
-      <c r="F324" s="5">
-        <v>1</v>
-      </c>
-      <c r="G324" s="5">
-        <v>0</v>
-      </c>
-      <c r="H324" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="I324" s="5" t="s">
-        <v>723</v>
-      </c>
-      <c r="J324" s="5">
-        <v>4</v>
-      </c>
-      <c r="K324" s="5">
-        <v>0</v>
-      </c>
-      <c r="L324" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M324" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N324" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O324" s="6"/>
-      <c r="P324" s="8"/>
-      <c r="Q324" s="6"/>
-      <c r="R324" s="8"/>
-      <c r="S324" s="6"/>
-      <c r="T324" s="8"/>
-      <c r="U324" s="6"/>
-      <c r="V324" s="8"/>
-      <c r="W324" s="6"/>
-      <c r="X324" s="8"/>
-      <c r="Y324" s="6"/>
-      <c r="Z324" s="6">
-        <v>2</v>
-      </c>
-      <c r="AA324" s="6" t="s">
+      <c r="I323" s="2" t="s">
         <v>726</v>
       </c>
-      <c r="AB324" s="5"/>
-    </row>
-    <row r="325" spans="1:28" outlineLevel="1">
-      <c r="A325" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B325" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C325" s="5">
-        <v>200</v>
-      </c>
-      <c r="D325" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E325" s="5"/>
-      <c r="F325" s="5">
-        <v>1</v>
-      </c>
-      <c r="G325" s="5">
-        <v>0</v>
-      </c>
-      <c r="H325" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="I325" s="5" t="s">
-        <v>723</v>
-      </c>
-      <c r="J325" s="5">
-        <v>4</v>
-      </c>
-      <c r="K325" s="5">
-        <v>0</v>
-      </c>
-      <c r="L325" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M325" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N325" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O325" s="6"/>
-      <c r="P325" s="8"/>
-      <c r="Q325" s="6"/>
-      <c r="R325" s="8"/>
-      <c r="S325" s="6"/>
-      <c r="T325" s="8"/>
-      <c r="U325" s="6"/>
-      <c r="V325" s="8"/>
-      <c r="W325" s="6"/>
-      <c r="X325" s="8"/>
-      <c r="Y325" s="6"/>
-      <c r="Z325" s="6">
-        <v>3</v>
-      </c>
-      <c r="AA325" s="6" t="s">
+      <c r="J323" s="2">
+        <v>64</v>
+      </c>
+      <c r="K323" s="2">
+        <v>0</v>
+      </c>
+      <c r="L323" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M323" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="N323" s="4"/>
+      <c r="O323" s="2"/>
+      <c r="P323" s="4"/>
+      <c r="Q323" s="2"/>
+      <c r="R323" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="S323" s="2"/>
+      <c r="T323" s="4"/>
+      <c r="U323" s="2"/>
+      <c r="V323" s="4"/>
+      <c r="W323" s="2"/>
+      <c r="X323" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y323" s="2"/>
+      <c r="Z323" s="2"/>
+      <c r="AA323" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB323" s="2"/>
+    </row>
+    <row r="324" spans="1:28">
+      <c r="A324" s="2" t="s">
         <v>727</v>
       </c>
-      <c r="AB325" s="5"/>
-    </row>
-    <row r="326" spans="1:28" outlineLevel="1">
-      <c r="A326" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B326" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C326" s="5">
-        <v>200</v>
-      </c>
-      <c r="D326" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E326" s="5"/>
-      <c r="F326" s="5">
-        <v>1</v>
-      </c>
-      <c r="G326" s="5">
-        <v>0</v>
-      </c>
-      <c r="H326" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="I326" s="5" t="s">
-        <v>723</v>
-      </c>
-      <c r="J326" s="5">
-        <v>4</v>
-      </c>
-      <c r="K326" s="5">
-        <v>0</v>
-      </c>
-      <c r="L326" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M326" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N326" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O326" s="6"/>
-      <c r="P326" s="8"/>
-      <c r="Q326" s="6"/>
-      <c r="R326" s="8"/>
-      <c r="S326" s="6"/>
-      <c r="T326" s="8"/>
-      <c r="U326" s="6"/>
-      <c r="V326" s="8"/>
-      <c r="W326" s="6"/>
-      <c r="X326" s="8"/>
-      <c r="Y326" s="6"/>
-      <c r="Z326" s="6">
-        <v>4</v>
-      </c>
-      <c r="AA326" s="6" t="s">
+      <c r="B324" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="AB326" s="5"/>
-    </row>
-    <row r="327" spans="1:28" outlineLevel="1">
-      <c r="A327" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B327" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C327" s="5">
-        <v>200</v>
-      </c>
-      <c r="D327" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E327" s="5"/>
-      <c r="F327" s="5">
-        <v>1</v>
-      </c>
-      <c r="G327" s="5">
-        <v>0</v>
-      </c>
-      <c r="H327" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="I327" s="5" t="s">
-        <v>723</v>
-      </c>
-      <c r="J327" s="5">
-        <v>4</v>
-      </c>
-      <c r="K327" s="5">
-        <v>0</v>
-      </c>
-      <c r="L327" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M327" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N327" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O327" s="6"/>
-      <c r="P327" s="8"/>
-      <c r="Q327" s="6"/>
-      <c r="R327" s="8"/>
-      <c r="S327" s="6"/>
-      <c r="T327" s="8"/>
-      <c r="U327" s="6"/>
-      <c r="V327" s="8"/>
-      <c r="W327" s="6"/>
-      <c r="X327" s="8"/>
-      <c r="Y327" s="6"/>
-      <c r="Z327" s="6">
-        <v>5</v>
-      </c>
-      <c r="AA327" s="6" t="s">
+      <c r="C324" s="2">
+        <v>0</v>
+      </c>
+      <c r="D324" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E324" s="2"/>
+      <c r="F324" s="2">
+        <v>1</v>
+      </c>
+      <c r="G324" s="2">
+        <v>0</v>
+      </c>
+      <c r="H324" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="I324" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="J324" s="2">
+        <v>64</v>
+      </c>
+      <c r="K324" s="2">
+        <v>0</v>
+      </c>
+      <c r="L324" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M324" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="N324" s="4"/>
+      <c r="O324" s="2"/>
+      <c r="P324" s="4"/>
+      <c r="Q324" s="2"/>
+      <c r="R324" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="S324" s="2"/>
+      <c r="T324" s="4"/>
+      <c r="U324" s="2"/>
+      <c r="V324" s="4"/>
+      <c r="W324" s="2"/>
+      <c r="X324" s="3" t="s">
         <v>729</v>
       </c>
-      <c r="AB327" s="5"/>
-    </row>
-    <row r="328" spans="1:28" outlineLevel="1">
-      <c r="A328" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B328" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C328" s="5">
-        <v>200</v>
-      </c>
-      <c r="D328" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E328" s="5"/>
-      <c r="F328" s="5">
-        <v>1</v>
-      </c>
-      <c r="G328" s="5">
-        <v>0</v>
-      </c>
-      <c r="H328" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="I328" s="5" t="s">
-        <v>723</v>
-      </c>
-      <c r="J328" s="5">
-        <v>4</v>
-      </c>
-      <c r="K328" s="5">
-        <v>0</v>
-      </c>
-      <c r="L328" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M328" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N328" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O328" s="6"/>
-      <c r="P328" s="8"/>
-      <c r="Q328" s="6"/>
-      <c r="R328" s="8"/>
-      <c r="S328" s="6"/>
-      <c r="T328" s="8"/>
-      <c r="U328" s="6"/>
-      <c r="V328" s="8"/>
-      <c r="W328" s="6"/>
-      <c r="X328" s="8"/>
-      <c r="Y328" s="6"/>
-      <c r="Z328" s="6">
-        <v>6</v>
-      </c>
-      <c r="AA328" s="6" t="s">
-        <v>730</v>
-      </c>
-      <c r="AB328" s="5"/>
-    </row>
-    <row r="329" spans="1:28" outlineLevel="1">
-      <c r="A329" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B329" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C329" s="5">
-        <v>200</v>
-      </c>
-      <c r="D329" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E329" s="5"/>
-      <c r="F329" s="5">
-        <v>1</v>
-      </c>
-      <c r="G329" s="5">
-        <v>0</v>
-      </c>
-      <c r="H329" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="I329" s="5" t="s">
-        <v>723</v>
-      </c>
-      <c r="J329" s="5">
-        <v>4</v>
-      </c>
-      <c r="K329" s="5">
-        <v>0</v>
-      </c>
-      <c r="L329" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M329" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N329" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O329" s="6"/>
-      <c r="P329" s="8"/>
-      <c r="Q329" s="6"/>
-      <c r="R329" s="8"/>
-      <c r="S329" s="6"/>
-      <c r="T329" s="8"/>
-      <c r="U329" s="6"/>
-      <c r="V329" s="8"/>
-      <c r="W329" s="6"/>
-      <c r="X329" s="8"/>
-      <c r="Y329" s="6"/>
-      <c r="Z329" s="6">
-        <v>7</v>
-      </c>
-      <c r="AA329" s="6" t="s">
-        <v>731</v>
-      </c>
-      <c r="AB329" s="5"/>
-    </row>
-    <row r="330" spans="1:28" outlineLevel="1">
-      <c r="A330" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B330" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C330" s="5">
-        <v>200</v>
-      </c>
-      <c r="D330" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E330" s="5"/>
-      <c r="F330" s="5">
-        <v>1</v>
-      </c>
-      <c r="G330" s="5">
-        <v>0</v>
-      </c>
-      <c r="H330" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="I330" s="5" t="s">
-        <v>723</v>
-      </c>
-      <c r="J330" s="5">
-        <v>4</v>
-      </c>
-      <c r="K330" s="5">
-        <v>0</v>
-      </c>
-      <c r="L330" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M330" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N330" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O330" s="6"/>
-      <c r="P330" s="8"/>
-      <c r="Q330" s="6"/>
-      <c r="R330" s="8"/>
-      <c r="S330" s="6"/>
-      <c r="T330" s="8"/>
-      <c r="U330" s="6"/>
-      <c r="V330" s="8"/>
-      <c r="W330" s="6"/>
-      <c r="X330" s="8"/>
-      <c r="Y330" s="6"/>
-      <c r="Z330" s="6">
-        <v>8</v>
-      </c>
-      <c r="AA330" s="6" t="s">
-        <v>732</v>
-      </c>
-      <c r="AB330" s="5"/>
-    </row>
-    <row r="331" spans="1:28" outlineLevel="1">
-      <c r="A331" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B331" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C331" s="5">
-        <v>200</v>
-      </c>
-      <c r="D331" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E331" s="5"/>
-      <c r="F331" s="6">
-        <v>1</v>
-      </c>
-      <c r="G331" s="6">
-        <v>4</v>
-      </c>
-      <c r="H331" s="6" t="s">
-        <v>733</v>
-      </c>
-      <c r="I331" s="6" t="s">
-        <v>734</v>
-      </c>
-      <c r="J331" s="6">
-        <v>4</v>
-      </c>
-      <c r="K331" s="6">
-        <v>0</v>
-      </c>
-      <c r="L331" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M331" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N331" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O331" s="6"/>
-      <c r="P331" s="8"/>
-      <c r="Q331" s="6"/>
-      <c r="R331" s="8"/>
-      <c r="S331" s="6"/>
-      <c r="T331" s="8"/>
-      <c r="U331" s="6"/>
-      <c r="V331" s="8"/>
-      <c r="W331" s="6"/>
-      <c r="X331" s="8"/>
-      <c r="Y331" s="6"/>
-      <c r="Z331" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA331" s="6" t="s">
-        <v>724</v>
-      </c>
-      <c r="AB331" s="6"/>
-    </row>
-    <row r="332" spans="1:28" outlineLevel="1">
-      <c r="A332" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B332" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C332" s="5">
-        <v>200</v>
-      </c>
-      <c r="D332" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E332" s="5"/>
-      <c r="F332" s="5">
-        <v>1</v>
-      </c>
-      <c r="G332" s="5">
-        <v>4</v>
-      </c>
-      <c r="H332" s="5" t="s">
-        <v>733</v>
-      </c>
-      <c r="I332" s="5" t="s">
-        <v>734</v>
-      </c>
-      <c r="J332" s="5">
-        <v>4</v>
-      </c>
-      <c r="K332" s="5">
-        <v>0</v>
-      </c>
-      <c r="L332" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M332" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N332" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O332" s="6"/>
-      <c r="P332" s="8"/>
-      <c r="Q332" s="6"/>
-      <c r="R332" s="8"/>
-      <c r="S332" s="6"/>
-      <c r="T332" s="8"/>
-      <c r="U332" s="6"/>
-      <c r="V332" s="8"/>
-      <c r="W332" s="6"/>
-      <c r="X332" s="8"/>
-      <c r="Y332" s="6"/>
-      <c r="Z332" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA332" s="6" t="s">
-        <v>725</v>
-      </c>
-      <c r="AB332" s="5"/>
-    </row>
-    <row r="333" spans="1:28" outlineLevel="1">
-      <c r="A333" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B333" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C333" s="5">
-        <v>200</v>
-      </c>
-      <c r="D333" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E333" s="5"/>
-      <c r="F333" s="5">
-        <v>1</v>
-      </c>
-      <c r="G333" s="5">
-        <v>4</v>
-      </c>
-      <c r="H333" s="5" t="s">
-        <v>733</v>
-      </c>
-      <c r="I333" s="5" t="s">
-        <v>734</v>
-      </c>
-      <c r="J333" s="5">
-        <v>4</v>
-      </c>
-      <c r="K333" s="5">
-        <v>0</v>
-      </c>
-      <c r="L333" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M333" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N333" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O333" s="6"/>
-      <c r="P333" s="8"/>
-      <c r="Q333" s="6"/>
-      <c r="R333" s="8"/>
-      <c r="S333" s="6"/>
-      <c r="T333" s="8"/>
-      <c r="U333" s="6"/>
-      <c r="V333" s="8"/>
-      <c r="W333" s="6"/>
-      <c r="X333" s="8"/>
-      <c r="Y333" s="6"/>
-      <c r="Z333" s="6">
-        <v>2</v>
-      </c>
-      <c r="AA333" s="6" t="s">
-        <v>726</v>
-      </c>
-      <c r="AB333" s="5"/>
-    </row>
-    <row r="334" spans="1:28" outlineLevel="1">
-      <c r="A334" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B334" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C334" s="5">
-        <v>200</v>
-      </c>
-      <c r="D334" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E334" s="5"/>
-      <c r="F334" s="5">
-        <v>1</v>
-      </c>
-      <c r="G334" s="5">
-        <v>4</v>
-      </c>
-      <c r="H334" s="5" t="s">
-        <v>733</v>
-      </c>
-      <c r="I334" s="5" t="s">
-        <v>734</v>
-      </c>
-      <c r="J334" s="5">
-        <v>4</v>
-      </c>
-      <c r="K334" s="5">
-        <v>0</v>
-      </c>
-      <c r="L334" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M334" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N334" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O334" s="6"/>
-      <c r="P334" s="8"/>
-      <c r="Q334" s="6"/>
-      <c r="R334" s="8"/>
-      <c r="S334" s="6"/>
-      <c r="T334" s="8"/>
-      <c r="U334" s="6"/>
-      <c r="V334" s="8"/>
-      <c r="W334" s="6"/>
-      <c r="X334" s="8"/>
-      <c r="Y334" s="6"/>
-      <c r="Z334" s="6">
-        <v>3</v>
-      </c>
-      <c r="AA334" s="6" t="s">
-        <v>727</v>
-      </c>
-      <c r="AB334" s="5"/>
-    </row>
-    <row r="335" spans="1:28" outlineLevel="1">
-      <c r="A335" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B335" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C335" s="5">
-        <v>200</v>
-      </c>
-      <c r="D335" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E335" s="5"/>
-      <c r="F335" s="5">
-        <v>1</v>
-      </c>
-      <c r="G335" s="5">
-        <v>4</v>
-      </c>
-      <c r="H335" s="5" t="s">
-        <v>733</v>
-      </c>
-      <c r="I335" s="5" t="s">
-        <v>734</v>
-      </c>
-      <c r="J335" s="5">
-        <v>4</v>
-      </c>
-      <c r="K335" s="5">
-        <v>0</v>
-      </c>
-      <c r="L335" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M335" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N335" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O335" s="6"/>
-      <c r="P335" s="8"/>
-      <c r="Q335" s="6"/>
-      <c r="R335" s="8"/>
-      <c r="S335" s="6"/>
-      <c r="T335" s="8"/>
-      <c r="U335" s="6"/>
-      <c r="V335" s="8"/>
-      <c r="W335" s="6"/>
-      <c r="X335" s="8"/>
-      <c r="Y335" s="6"/>
-      <c r="Z335" s="6">
-        <v>4</v>
-      </c>
-      <c r="AA335" s="6" t="s">
-        <v>728</v>
-      </c>
-      <c r="AB335" s="5"/>
-    </row>
-    <row r="336" spans="1:28" outlineLevel="1">
-      <c r="A336" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B336" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C336" s="5">
-        <v>200</v>
-      </c>
-      <c r="D336" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E336" s="5"/>
-      <c r="F336" s="5">
-        <v>1</v>
-      </c>
-      <c r="G336" s="5">
-        <v>4</v>
-      </c>
-      <c r="H336" s="5" t="s">
-        <v>733</v>
-      </c>
-      <c r="I336" s="5" t="s">
-        <v>734</v>
-      </c>
-      <c r="J336" s="5">
-        <v>4</v>
-      </c>
-      <c r="K336" s="5">
-        <v>0</v>
-      </c>
-      <c r="L336" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M336" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N336" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O336" s="6"/>
-      <c r="P336" s="8"/>
-      <c r="Q336" s="6"/>
-      <c r="R336" s="8"/>
-      <c r="S336" s="6"/>
-      <c r="T336" s="8"/>
-      <c r="U336" s="6"/>
-      <c r="V336" s="8"/>
-      <c r="W336" s="6"/>
-      <c r="X336" s="8"/>
-      <c r="Y336" s="6"/>
-      <c r="Z336" s="6">
-        <v>5</v>
-      </c>
-      <c r="AA336" s="6" t="s">
-        <v>729</v>
-      </c>
-      <c r="AB336" s="5"/>
-    </row>
-    <row r="337" spans="1:28" outlineLevel="1">
-      <c r="A337" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B337" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C337" s="5">
-        <v>200</v>
-      </c>
-      <c r="D337" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E337" s="5"/>
-      <c r="F337" s="5">
-        <v>1</v>
-      </c>
-      <c r="G337" s="5">
-        <v>4</v>
-      </c>
-      <c r="H337" s="5" t="s">
-        <v>733</v>
-      </c>
-      <c r="I337" s="5" t="s">
-        <v>734</v>
-      </c>
-      <c r="J337" s="5">
-        <v>4</v>
-      </c>
-      <c r="K337" s="5">
-        <v>0</v>
-      </c>
-      <c r="L337" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M337" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N337" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O337" s="6"/>
-      <c r="P337" s="8"/>
-      <c r="Q337" s="6"/>
-      <c r="R337" s="8"/>
-      <c r="S337" s="6"/>
-      <c r="T337" s="8"/>
-      <c r="U337" s="6"/>
-      <c r="V337" s="8"/>
-      <c r="W337" s="6"/>
-      <c r="X337" s="8"/>
-      <c r="Y337" s="6"/>
-      <c r="Z337" s="6">
-        <v>6</v>
-      </c>
-      <c r="AA337" s="6" t="s">
-        <v>730</v>
-      </c>
-      <c r="AB337" s="5"/>
-    </row>
-    <row r="338" spans="1:28" outlineLevel="1">
-      <c r="A338" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B338" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C338" s="5">
-        <v>200</v>
-      </c>
-      <c r="D338" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E338" s="5"/>
-      <c r="F338" s="5">
-        <v>1</v>
-      </c>
-      <c r="G338" s="5">
-        <v>4</v>
-      </c>
-      <c r="H338" s="5" t="s">
-        <v>733</v>
-      </c>
-      <c r="I338" s="5" t="s">
-        <v>734</v>
-      </c>
-      <c r="J338" s="5">
-        <v>4</v>
-      </c>
-      <c r="K338" s="5">
-        <v>0</v>
-      </c>
-      <c r="L338" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M338" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N338" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O338" s="6"/>
-      <c r="P338" s="8"/>
-      <c r="Q338" s="6"/>
-      <c r="R338" s="8"/>
-      <c r="S338" s="6"/>
-      <c r="T338" s="8"/>
-      <c r="U338" s="6"/>
-      <c r="V338" s="8"/>
-      <c r="W338" s="6"/>
-      <c r="X338" s="8"/>
-      <c r="Y338" s="6"/>
-      <c r="Z338" s="6">
-        <v>7</v>
-      </c>
-      <c r="AA338" s="6" t="s">
-        <v>731</v>
-      </c>
-      <c r="AB338" s="5"/>
-    </row>
-    <row r="339" spans="1:28" outlineLevel="1">
-      <c r="A339" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B339" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C339" s="5">
-        <v>200</v>
-      </c>
-      <c r="D339" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E339" s="5"/>
-      <c r="F339" s="5">
-        <v>1</v>
-      </c>
-      <c r="G339" s="5">
-        <v>4</v>
-      </c>
-      <c r="H339" s="5" t="s">
-        <v>733</v>
-      </c>
-      <c r="I339" s="5" t="s">
-        <v>734</v>
-      </c>
-      <c r="J339" s="5">
-        <v>4</v>
-      </c>
-      <c r="K339" s="5">
-        <v>0</v>
-      </c>
-      <c r="L339" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M339" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N339" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O339" s="6"/>
-      <c r="P339" s="8"/>
-      <c r="Q339" s="6"/>
-      <c r="R339" s="8"/>
-      <c r="S339" s="6"/>
-      <c r="T339" s="8"/>
-      <c r="U339" s="6"/>
-      <c r="V339" s="8"/>
-      <c r="W339" s="6"/>
-      <c r="X339" s="8"/>
-      <c r="Y339" s="6"/>
-      <c r="Z339" s="6">
-        <v>8</v>
-      </c>
-      <c r="AA339" s="6" t="s">
-        <v>732</v>
-      </c>
-      <c r="AB339" s="5"/>
-    </row>
-    <row r="340" spans="1:28" outlineLevel="1">
-      <c r="A340" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B340" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C340" s="5">
-        <v>200</v>
-      </c>
-      <c r="D340" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E340" s="5"/>
-      <c r="F340" s="6">
-        <v>2</v>
-      </c>
-      <c r="G340" s="6">
-        <v>0</v>
-      </c>
-      <c r="H340" s="6" t="s">
-        <v>735</v>
-      </c>
-      <c r="I340" s="6" t="s">
-        <v>736</v>
-      </c>
-      <c r="J340" s="6">
-        <v>4</v>
-      </c>
-      <c r="K340" s="6">
-        <v>0</v>
-      </c>
-      <c r="L340" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M340" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N340" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O340" s="6"/>
-      <c r="P340" s="8"/>
-      <c r="Q340" s="6"/>
-      <c r="R340" s="8"/>
-      <c r="S340" s="6"/>
-      <c r="T340" s="8"/>
-      <c r="U340" s="6"/>
-      <c r="V340" s="8"/>
-      <c r="W340" s="6"/>
-      <c r="X340" s="8"/>
-      <c r="Y340" s="6"/>
-      <c r="Z340" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA340" s="6" t="s">
-        <v>724</v>
-      </c>
-      <c r="AB340" s="6"/>
-    </row>
-    <row r="341" spans="1:28" outlineLevel="1">
-      <c r="A341" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B341" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C341" s="5">
-        <v>200</v>
-      </c>
-      <c r="D341" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E341" s="5"/>
-      <c r="F341" s="5">
-        <v>2</v>
-      </c>
-      <c r="G341" s="5">
-        <v>0</v>
-      </c>
-      <c r="H341" s="5" t="s">
-        <v>735</v>
-      </c>
-      <c r="I341" s="5" t="s">
-        <v>736</v>
-      </c>
-      <c r="J341" s="5">
-        <v>4</v>
-      </c>
-      <c r="K341" s="5">
-        <v>0</v>
-      </c>
-      <c r="L341" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M341" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N341" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O341" s="6"/>
-      <c r="P341" s="8"/>
-      <c r="Q341" s="6"/>
-      <c r="R341" s="8"/>
-      <c r="S341" s="6"/>
-      <c r="T341" s="8"/>
-      <c r="U341" s="6"/>
-      <c r="V341" s="8"/>
-      <c r="W341" s="6"/>
-      <c r="X341" s="8"/>
-      <c r="Y341" s="6"/>
-      <c r="Z341" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA341" s="6" t="s">
-        <v>725</v>
-      </c>
-      <c r="AB341" s="5"/>
-    </row>
-    <row r="342" spans="1:28" outlineLevel="1">
-      <c r="A342" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B342" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C342" s="5">
-        <v>200</v>
-      </c>
-      <c r="D342" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E342" s="5"/>
-      <c r="F342" s="5">
-        <v>2</v>
-      </c>
-      <c r="G342" s="5">
-        <v>0</v>
-      </c>
-      <c r="H342" s="5" t="s">
-        <v>735</v>
-      </c>
-      <c r="I342" s="5" t="s">
-        <v>736</v>
-      </c>
-      <c r="J342" s="5">
-        <v>4</v>
-      </c>
-      <c r="K342" s="5">
-        <v>0</v>
-      </c>
-      <c r="L342" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M342" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N342" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O342" s="6"/>
-      <c r="P342" s="8"/>
-      <c r="Q342" s="6"/>
-      <c r="R342" s="8"/>
-      <c r="S342" s="6"/>
-      <c r="T342" s="8"/>
-      <c r="U342" s="6"/>
-      <c r="V342" s="8"/>
-      <c r="W342" s="6"/>
-      <c r="X342" s="8"/>
-      <c r="Y342" s="6"/>
-      <c r="Z342" s="6">
-        <v>2</v>
-      </c>
-      <c r="AA342" s="6" t="s">
-        <v>726</v>
-      </c>
-      <c r="AB342" s="5"/>
-    </row>
-    <row r="343" spans="1:28" outlineLevel="1">
-      <c r="A343" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B343" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C343" s="5">
-        <v>200</v>
-      </c>
-      <c r="D343" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E343" s="5"/>
-      <c r="F343" s="5">
-        <v>2</v>
-      </c>
-      <c r="G343" s="5">
-        <v>0</v>
-      </c>
-      <c r="H343" s="5" t="s">
-        <v>735</v>
-      </c>
-      <c r="I343" s="5" t="s">
-        <v>736</v>
-      </c>
-      <c r="J343" s="5">
-        <v>4</v>
-      </c>
-      <c r="K343" s="5">
-        <v>0</v>
-      </c>
-      <c r="L343" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M343" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N343" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O343" s="6"/>
-      <c r="P343" s="8"/>
-      <c r="Q343" s="6"/>
-      <c r="R343" s="8"/>
-      <c r="S343" s="6"/>
-      <c r="T343" s="8"/>
-      <c r="U343" s="6"/>
-      <c r="V343" s="8"/>
-      <c r="W343" s="6"/>
-      <c r="X343" s="8"/>
-      <c r="Y343" s="6"/>
-      <c r="Z343" s="6">
-        <v>3</v>
-      </c>
-      <c r="AA343" s="6" t="s">
-        <v>727</v>
-      </c>
-      <c r="AB343" s="5"/>
-    </row>
-    <row r="344" spans="1:28" outlineLevel="1">
-      <c r="A344" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B344" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C344" s="5">
-        <v>200</v>
-      </c>
-      <c r="D344" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E344" s="5"/>
-      <c r="F344" s="5">
-        <v>2</v>
-      </c>
-      <c r="G344" s="5">
-        <v>0</v>
-      </c>
-      <c r="H344" s="5" t="s">
-        <v>735</v>
-      </c>
-      <c r="I344" s="5" t="s">
-        <v>736</v>
-      </c>
-      <c r="J344" s="5">
-        <v>4</v>
-      </c>
-      <c r="K344" s="5">
-        <v>0</v>
-      </c>
-      <c r="L344" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M344" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N344" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O344" s="6"/>
-      <c r="P344" s="8"/>
-      <c r="Q344" s="6"/>
-      <c r="R344" s="8"/>
-      <c r="S344" s="6"/>
-      <c r="T344" s="8"/>
-      <c r="U344" s="6"/>
-      <c r="V344" s="8"/>
-      <c r="W344" s="6"/>
-      <c r="X344" s="8"/>
-      <c r="Y344" s="6"/>
-      <c r="Z344" s="6">
-        <v>4</v>
-      </c>
-      <c r="AA344" s="6" t="s">
-        <v>728</v>
-      </c>
-      <c r="AB344" s="5"/>
-    </row>
-    <row r="345" spans="1:28" outlineLevel="1">
-      <c r="A345" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B345" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C345" s="5">
-        <v>200</v>
-      </c>
-      <c r="D345" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E345" s="5"/>
-      <c r="F345" s="5">
-        <v>2</v>
-      </c>
-      <c r="G345" s="5">
-        <v>0</v>
-      </c>
-      <c r="H345" s="5" t="s">
-        <v>735</v>
-      </c>
-      <c r="I345" s="5" t="s">
-        <v>736</v>
-      </c>
-      <c r="J345" s="5">
-        <v>4</v>
-      </c>
-      <c r="K345" s="5">
-        <v>0</v>
-      </c>
-      <c r="L345" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M345" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N345" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O345" s="6"/>
-      <c r="P345" s="8"/>
-      <c r="Q345" s="6"/>
-      <c r="R345" s="8"/>
-      <c r="S345" s="6"/>
-      <c r="T345" s="8"/>
-      <c r="U345" s="6"/>
-      <c r="V345" s="8"/>
-      <c r="W345" s="6"/>
-      <c r="X345" s="8"/>
-      <c r="Y345" s="6"/>
-      <c r="Z345" s="6">
-        <v>5</v>
-      </c>
-      <c r="AA345" s="6" t="s">
-        <v>729</v>
-      </c>
-      <c r="AB345" s="5"/>
-    </row>
-    <row r="346" spans="1:28" outlineLevel="1">
-      <c r="A346" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B346" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C346" s="5">
-        <v>200</v>
-      </c>
-      <c r="D346" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E346" s="5"/>
-      <c r="F346" s="5">
-        <v>2</v>
-      </c>
-      <c r="G346" s="5">
-        <v>0</v>
-      </c>
-      <c r="H346" s="5" t="s">
-        <v>735</v>
-      </c>
-      <c r="I346" s="5" t="s">
-        <v>736</v>
-      </c>
-      <c r="J346" s="5">
-        <v>4</v>
-      </c>
-      <c r="K346" s="5">
-        <v>0</v>
-      </c>
-      <c r="L346" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M346" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N346" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O346" s="6"/>
-      <c r="P346" s="8"/>
-      <c r="Q346" s="6"/>
-      <c r="R346" s="8"/>
-      <c r="S346" s="6"/>
-      <c r="T346" s="8"/>
-      <c r="U346" s="6"/>
-      <c r="V346" s="8"/>
-      <c r="W346" s="6"/>
-      <c r="X346" s="8"/>
-      <c r="Y346" s="6"/>
-      <c r="Z346" s="6">
-        <v>6</v>
-      </c>
-      <c r="AA346" s="6" t="s">
-        <v>730</v>
-      </c>
-      <c r="AB346" s="5"/>
-    </row>
-    <row r="347" spans="1:28" outlineLevel="1">
-      <c r="A347" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B347" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C347" s="5">
-        <v>200</v>
-      </c>
-      <c r="D347" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E347" s="5"/>
-      <c r="F347" s="5">
-        <v>2</v>
-      </c>
-      <c r="G347" s="5">
-        <v>0</v>
-      </c>
-      <c r="H347" s="5" t="s">
-        <v>735</v>
-      </c>
-      <c r="I347" s="5" t="s">
-        <v>736</v>
-      </c>
-      <c r="J347" s="5">
-        <v>4</v>
-      </c>
-      <c r="K347" s="5">
-        <v>0</v>
-      </c>
-      <c r="L347" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M347" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N347" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O347" s="6"/>
-      <c r="P347" s="8"/>
-      <c r="Q347" s="6"/>
-      <c r="R347" s="8"/>
-      <c r="S347" s="6"/>
-      <c r="T347" s="8"/>
-      <c r="U347" s="6"/>
-      <c r="V347" s="8"/>
-      <c r="W347" s="6"/>
-      <c r="X347" s="8"/>
-      <c r="Y347" s="6"/>
-      <c r="Z347" s="6">
-        <v>7</v>
-      </c>
-      <c r="AA347" s="6" t="s">
-        <v>731</v>
-      </c>
-      <c r="AB347" s="5"/>
-    </row>
-    <row r="348" spans="1:28" outlineLevel="1">
-      <c r="A348" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B348" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C348" s="5">
-        <v>200</v>
-      </c>
-      <c r="D348" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E348" s="5"/>
-      <c r="F348" s="5">
-        <v>2</v>
-      </c>
-      <c r="G348" s="5">
-        <v>0</v>
-      </c>
-      <c r="H348" s="5" t="s">
-        <v>735</v>
-      </c>
-      <c r="I348" s="5" t="s">
-        <v>736</v>
-      </c>
-      <c r="J348" s="5">
-        <v>4</v>
-      </c>
-      <c r="K348" s="5">
-        <v>0</v>
-      </c>
-      <c r="L348" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M348" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N348" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O348" s="6"/>
-      <c r="P348" s="8"/>
-      <c r="Q348" s="6"/>
-      <c r="R348" s="8"/>
-      <c r="S348" s="6"/>
-      <c r="T348" s="8"/>
-      <c r="U348" s="6"/>
-      <c r="V348" s="8"/>
-      <c r="W348" s="6"/>
-      <c r="X348" s="8"/>
-      <c r="Y348" s="6"/>
-      <c r="Z348" s="6">
-        <v>8</v>
-      </c>
-      <c r="AA348" s="6" t="s">
-        <v>732</v>
-      </c>
-      <c r="AB348" s="5"/>
-    </row>
-    <row r="349" spans="1:28" outlineLevel="1">
-      <c r="A349" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B349" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C349" s="5">
-        <v>200</v>
-      </c>
-      <c r="D349" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E349" s="5"/>
-      <c r="F349" s="6">
-        <v>2</v>
-      </c>
-      <c r="G349" s="6">
-        <v>4</v>
-      </c>
-      <c r="H349" s="6" t="s">
-        <v>737</v>
-      </c>
-      <c r="I349" s="6" t="s">
-        <v>738</v>
-      </c>
-      <c r="J349" s="6">
-        <v>4</v>
-      </c>
-      <c r="K349" s="6">
-        <v>0</v>
-      </c>
-      <c r="L349" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M349" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N349" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O349" s="6"/>
-      <c r="P349" s="8"/>
-      <c r="Q349" s="6"/>
-      <c r="R349" s="8"/>
-      <c r="S349" s="6"/>
-      <c r="T349" s="8"/>
-      <c r="U349" s="6"/>
-      <c r="V349" s="8"/>
-      <c r="W349" s="6"/>
-      <c r="X349" s="8"/>
-      <c r="Y349" s="6"/>
-      <c r="Z349" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA349" s="6" t="s">
-        <v>724</v>
-      </c>
-      <c r="AB349" s="6"/>
-    </row>
-    <row r="350" spans="1:28" outlineLevel="1">
-      <c r="A350" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B350" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C350" s="5">
-        <v>200</v>
-      </c>
-      <c r="D350" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E350" s="5"/>
-      <c r="F350" s="5">
-        <v>2</v>
-      </c>
-      <c r="G350" s="5">
-        <v>4</v>
-      </c>
-      <c r="H350" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="I350" s="5" t="s">
-        <v>738</v>
-      </c>
-      <c r="J350" s="5">
-        <v>4</v>
-      </c>
-      <c r="K350" s="5">
-        <v>0</v>
-      </c>
-      <c r="L350" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M350" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N350" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O350" s="6"/>
-      <c r="P350" s="8"/>
-      <c r="Q350" s="6"/>
-      <c r="R350" s="8"/>
-      <c r="S350" s="6"/>
-      <c r="T350" s="8"/>
-      <c r="U350" s="6"/>
-      <c r="V350" s="8"/>
-      <c r="W350" s="6"/>
-      <c r="X350" s="8"/>
-      <c r="Y350" s="6"/>
-      <c r="Z350" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA350" s="6" t="s">
-        <v>725</v>
-      </c>
-      <c r="AB350" s="5"/>
-    </row>
-    <row r="351" spans="1:28" outlineLevel="1">
-      <c r="A351" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B351" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C351" s="5">
-        <v>200</v>
-      </c>
-      <c r="D351" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E351" s="5"/>
-      <c r="F351" s="5">
-        <v>2</v>
-      </c>
-      <c r="G351" s="5">
-        <v>4</v>
-      </c>
-      <c r="H351" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="I351" s="5" t="s">
-        <v>738</v>
-      </c>
-      <c r="J351" s="5">
-        <v>4</v>
-      </c>
-      <c r="K351" s="5">
-        <v>0</v>
-      </c>
-      <c r="L351" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M351" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N351" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O351" s="6"/>
-      <c r="P351" s="8"/>
-      <c r="Q351" s="6"/>
-      <c r="R351" s="8"/>
-      <c r="S351" s="6"/>
-      <c r="T351" s="8"/>
-      <c r="U351" s="6"/>
-      <c r="V351" s="8"/>
-      <c r="W351" s="6"/>
-      <c r="X351" s="8"/>
-      <c r="Y351" s="6"/>
-      <c r="Z351" s="6">
-        <v>2</v>
-      </c>
-      <c r="AA351" s="6" t="s">
-        <v>726</v>
-      </c>
-      <c r="AB351" s="5"/>
-    </row>
-    <row r="352" spans="1:28" outlineLevel="1">
-      <c r="A352" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B352" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C352" s="5">
-        <v>200</v>
-      </c>
-      <c r="D352" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E352" s="5"/>
-      <c r="F352" s="5">
-        <v>2</v>
-      </c>
-      <c r="G352" s="5">
-        <v>4</v>
-      </c>
-      <c r="H352" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="I352" s="5" t="s">
-        <v>738</v>
-      </c>
-      <c r="J352" s="5">
-        <v>4</v>
-      </c>
-      <c r="K352" s="5">
-        <v>0</v>
-      </c>
-      <c r="L352" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M352" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N352" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O352" s="6"/>
-      <c r="P352" s="8"/>
-      <c r="Q352" s="6"/>
-      <c r="R352" s="8"/>
-      <c r="S352" s="6"/>
-      <c r="T352" s="8"/>
-      <c r="U352" s="6"/>
-      <c r="V352" s="8"/>
-      <c r="W352" s="6"/>
-      <c r="X352" s="8"/>
-      <c r="Y352" s="6"/>
-      <c r="Z352" s="6">
-        <v>3</v>
-      </c>
-      <c r="AA352" s="6" t="s">
-        <v>727</v>
-      </c>
-      <c r="AB352" s="5"/>
-    </row>
-    <row r="353" spans="1:28" outlineLevel="1">
-      <c r="A353" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B353" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C353" s="5">
-        <v>200</v>
-      </c>
-      <c r="D353" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E353" s="5"/>
-      <c r="F353" s="5">
-        <v>2</v>
-      </c>
-      <c r="G353" s="5">
-        <v>4</v>
-      </c>
-      <c r="H353" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="I353" s="5" t="s">
-        <v>738</v>
-      </c>
-      <c r="J353" s="5">
-        <v>4</v>
-      </c>
-      <c r="K353" s="5">
-        <v>0</v>
-      </c>
-      <c r="L353" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M353" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N353" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O353" s="6"/>
-      <c r="P353" s="8"/>
-      <c r="Q353" s="6"/>
-      <c r="R353" s="8"/>
-      <c r="S353" s="6"/>
-      <c r="T353" s="8"/>
-      <c r="U353" s="6"/>
-      <c r="V353" s="8"/>
-      <c r="W353" s="6"/>
-      <c r="X353" s="8"/>
-      <c r="Y353" s="6"/>
-      <c r="Z353" s="6">
-        <v>4</v>
-      </c>
-      <c r="AA353" s="6" t="s">
-        <v>728</v>
-      </c>
-      <c r="AB353" s="5"/>
-    </row>
-    <row r="354" spans="1:28" outlineLevel="1">
-      <c r="A354" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B354" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C354" s="5">
-        <v>200</v>
-      </c>
-      <c r="D354" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E354" s="5"/>
-      <c r="F354" s="5">
-        <v>2</v>
-      </c>
-      <c r="G354" s="5">
-        <v>4</v>
-      </c>
-      <c r="H354" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="I354" s="5" t="s">
-        <v>738</v>
-      </c>
-      <c r="J354" s="5">
-        <v>4</v>
-      </c>
-      <c r="K354" s="5">
-        <v>0</v>
-      </c>
-      <c r="L354" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M354" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N354" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O354" s="6"/>
-      <c r="P354" s="8"/>
-      <c r="Q354" s="6"/>
-      <c r="R354" s="8"/>
-      <c r="S354" s="6"/>
-      <c r="T354" s="8"/>
-      <c r="U354" s="6"/>
-      <c r="V354" s="8"/>
-      <c r="W354" s="6"/>
-      <c r="X354" s="8"/>
-      <c r="Y354" s="6"/>
-      <c r="Z354" s="6">
-        <v>5</v>
-      </c>
-      <c r="AA354" s="6" t="s">
-        <v>729</v>
-      </c>
-      <c r="AB354" s="5"/>
-    </row>
-    <row r="355" spans="1:28" outlineLevel="1">
-      <c r="A355" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B355" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C355" s="5">
-        <v>200</v>
-      </c>
-      <c r="D355" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E355" s="5"/>
-      <c r="F355" s="5">
-        <v>2</v>
-      </c>
-      <c r="G355" s="5">
-        <v>4</v>
-      </c>
-      <c r="H355" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="I355" s="5" t="s">
-        <v>738</v>
-      </c>
-      <c r="J355" s="5">
-        <v>4</v>
-      </c>
-      <c r="K355" s="5">
-        <v>0</v>
-      </c>
-      <c r="L355" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M355" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N355" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O355" s="6"/>
-      <c r="P355" s="8"/>
-      <c r="Q355" s="6"/>
-      <c r="R355" s="8"/>
-      <c r="S355" s="6"/>
-      <c r="T355" s="8"/>
-      <c r="U355" s="6"/>
-      <c r="V355" s="8"/>
-      <c r="W355" s="6"/>
-      <c r="X355" s="8"/>
-      <c r="Y355" s="6"/>
-      <c r="Z355" s="6">
-        <v>6</v>
-      </c>
-      <c r="AA355" s="6" t="s">
-        <v>730</v>
-      </c>
-      <c r="AB355" s="5"/>
-    </row>
-    <row r="356" spans="1:28" outlineLevel="1">
-      <c r="A356" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B356" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C356" s="5">
-        <v>200</v>
-      </c>
-      <c r="D356" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E356" s="5"/>
-      <c r="F356" s="5">
-        <v>2</v>
-      </c>
-      <c r="G356" s="5">
-        <v>4</v>
-      </c>
-      <c r="H356" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="I356" s="5" t="s">
-        <v>738</v>
-      </c>
-      <c r="J356" s="5">
-        <v>4</v>
-      </c>
-      <c r="K356" s="5">
-        <v>0</v>
-      </c>
-      <c r="L356" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M356" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N356" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O356" s="6"/>
-      <c r="P356" s="8"/>
-      <c r="Q356" s="6"/>
-      <c r="R356" s="8"/>
-      <c r="S356" s="6"/>
-      <c r="T356" s="8"/>
-      <c r="U356" s="6"/>
-      <c r="V356" s="8"/>
-      <c r="W356" s="6"/>
-      <c r="X356" s="8"/>
-      <c r="Y356" s="6"/>
-      <c r="Z356" s="6">
-        <v>7</v>
-      </c>
-      <c r="AA356" s="6" t="s">
-        <v>731</v>
-      </c>
-      <c r="AB356" s="5"/>
-    </row>
-    <row r="357" spans="1:28" outlineLevel="1">
-      <c r="A357" s="5" t="s">
-        <v>720</v>
-      </c>
-      <c r="B357" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="C357" s="5">
-        <v>200</v>
-      </c>
-      <c r="D357" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E357" s="5"/>
-      <c r="F357" s="5">
-        <v>2</v>
-      </c>
-      <c r="G357" s="5">
-        <v>4</v>
-      </c>
-      <c r="H357" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="I357" s="5" t="s">
-        <v>738</v>
-      </c>
-      <c r="J357" s="5">
-        <v>4</v>
-      </c>
-      <c r="K357" s="5">
-        <v>0</v>
-      </c>
-      <c r="L357" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M357" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N357" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O357" s="6"/>
-      <c r="P357" s="8"/>
-      <c r="Q357" s="6"/>
-      <c r="R357" s="8"/>
-      <c r="S357" s="6"/>
-      <c r="T357" s="8"/>
-      <c r="U357" s="6"/>
-      <c r="V357" s="8"/>
-      <c r="W357" s="6"/>
-      <c r="X357" s="8"/>
-      <c r="Y357" s="6"/>
-      <c r="Z357" s="6">
-        <v>8</v>
-      </c>
-      <c r="AA357" s="6" t="s">
-        <v>732</v>
-      </c>
-      <c r="AB357" s="5"/>
-    </row>
-    <row r="358" spans="1:28">
-      <c r="A358" s="2" t="s">
-        <v>739</v>
-      </c>
-      <c r="B358" s="2" t="s">
-        <v>740</v>
-      </c>
-      <c r="C358" s="2">
-        <v>0</v>
-      </c>
-      <c r="D358" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E358" s="2"/>
-      <c r="F358" s="2">
-        <v>1</v>
-      </c>
-      <c r="G358" s="2">
-        <v>0</v>
-      </c>
-      <c r="H358" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="I358" s="2"/>
-      <c r="J358" s="2">
-        <v>64</v>
-      </c>
-      <c r="K358" s="2">
-        <v>0</v>
-      </c>
-      <c r="L358" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M358" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N358" s="4"/>
-      <c r="O358" s="2"/>
-      <c r="P358" s="4"/>
-      <c r="Q358" s="2"/>
-      <c r="R358" s="4"/>
-      <c r="S358" s="2"/>
-      <c r="T358" s="4"/>
-      <c r="U358" s="2"/>
-      <c r="V358" s="4"/>
-      <c r="W358" s="2"/>
-      <c r="X358" s="4"/>
-      <c r="Y358" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z358" s="2"/>
-      <c r="AA358" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB358" s="2"/>
-    </row>
-    <row r="359" spans="1:28">
-      <c r="A359" s="2" t="s">
-        <v>742</v>
-      </c>
-      <c r="B359" s="2" t="s">
-        <v>743</v>
-      </c>
-      <c r="C359" s="2">
-        <v>0</v>
-      </c>
-      <c r="D359" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E359" s="2"/>
-      <c r="F359" s="2">
-        <v>1</v>
-      </c>
-      <c r="G359" s="2">
-        <v>0</v>
-      </c>
-      <c r="H359" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="I359" s="2" t="s">
-        <v>745</v>
-      </c>
-      <c r="J359" s="2">
-        <v>64</v>
-      </c>
-      <c r="K359" s="2">
-        <v>0</v>
-      </c>
-      <c r="L359" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M359" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="N359" s="4"/>
-      <c r="O359" s="2"/>
-      <c r="P359" s="4"/>
-      <c r="Q359" s="2"/>
-      <c r="R359" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="S359" s="2"/>
-      <c r="T359" s="4"/>
-      <c r="U359" s="2"/>
-      <c r="V359" s="4"/>
-      <c r="W359" s="2"/>
-      <c r="X359" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y359" s="2"/>
-      <c r="Z359" s="2"/>
-      <c r="AA359" s="2" t="s">
+      <c r="Y324" s="2"/>
+      <c r="Z324" s="2"/>
+      <c r="AA324" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="AB359" s="2"/>
-    </row>
-    <row r="360" spans="1:28">
-      <c r="A360" s="2" t="s">
-        <v>746</v>
-      </c>
-      <c r="B360" s="2" t="s">
-        <v>747</v>
-      </c>
-      <c r="C360" s="2">
-        <v>0</v>
-      </c>
-      <c r="D360" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E360" s="2"/>
-      <c r="F360" s="2">
-        <v>1</v>
-      </c>
-      <c r="G360" s="2">
-        <v>0</v>
-      </c>
-      <c r="H360" s="2" t="s">
-        <v>749</v>
-      </c>
-      <c r="I360" s="2" t="s">
-        <v>750</v>
-      </c>
-      <c r="J360" s="2">
-        <v>64</v>
-      </c>
-      <c r="K360" s="2">
-        <v>0</v>
-      </c>
-      <c r="L360" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M360" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="N360" s="4"/>
-      <c r="O360" s="2"/>
-      <c r="P360" s="4"/>
-      <c r="Q360" s="2"/>
-      <c r="R360" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="S360" s="2"/>
-      <c r="T360" s="4"/>
-      <c r="U360" s="2"/>
-      <c r="V360" s="4"/>
-      <c r="W360" s="2"/>
-      <c r="X360" s="3" t="s">
-        <v>748</v>
-      </c>
-      <c r="Y360" s="2"/>
-      <c r="Z360" s="2"/>
-      <c r="AA360" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="AB360" s="2"/>
+      <c r="AB324" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AR361"/>
+  <autoFilter ref="A1:AR325"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>